<commit_message>
Missing figures in simulation and the whole results and conclusion
</commit_message>
<xml_diff>
--- a/EJ2/Mediciones/Mediciones tp2 ej2 Zin LM833.xlsx
+++ b/EJ2/Mediciones/Mediciones tp2 ej2 Zin LM833.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\facun\OneDrive\Desktop\ITBA\5C TC\TP2\TP2\EJ2\Mediciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016D0CD2-2DEE-4050-91EC-B0FB24E66120}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41897141-B1B5-42FF-979D-A03E6467FE72}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{725EB9F4-FAC7-4A66-873D-D6BC0385B064}"/>
   </bookViews>
@@ -50,10 +50,10 @@
     <t>Zin (Ohm)</t>
   </si>
   <si>
-    <t>Frec (KHz)</t>
+    <t>Vpp serie (mV)</t>
   </si>
   <si>
-    <t>Vpp serie (mV)</t>
+    <t>Frec (Hz)</t>
   </si>
 </sst>
 </file>
@@ -210,58 +210,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="114"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>25000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>35000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>75</c:v>
+                  <c:v>75000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>85</c:v>
+                  <c:v>85000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>130</c:v>
+                  <c:v>130000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>200</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>250</c:v>
+                  <c:v>250000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>500</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -878,58 +878,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="114"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>25000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>35000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>75</c:v>
+                  <c:v>75000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>85</c:v>
+                  <c:v>85000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>130</c:v>
+                  <c:v>130000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>200</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>250</c:v>
+                  <c:v>250000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>500</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2675,7 +2675,7 @@
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2690,13 +2690,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -2738,7 +2738,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>8</v>
+        <v>8000</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -2763,7 +2763,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="B4">
         <v>200</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>20</v>
+        <v>20000</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -2813,7 +2813,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="B6">
         <v>200</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>30</v>
+        <v>30000</v>
       </c>
       <c r="B7">
         <v>200</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>35</v>
+        <v>35000</v>
       </c>
       <c r="B8">
         <v>200</v>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>40</v>
+        <v>40000</v>
       </c>
       <c r="B9">
         <v>200</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>45</v>
+        <v>45000</v>
       </c>
       <c r="B10">
         <v>200</v>
@@ -2938,7 +2938,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>50</v>
+        <v>50000</v>
       </c>
       <c r="B11">
         <v>200</v>
@@ -2963,7 +2963,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>60</v>
+        <v>60000</v>
       </c>
       <c r="B12">
         <v>200</v>
@@ -2988,7 +2988,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="B13">
         <v>200</v>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>85</v>
+        <v>85000</v>
       </c>
       <c r="B14">
         <v>200</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="B15">
         <v>200</v>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>130</v>
+        <v>130000</v>
       </c>
       <c r="B16">
         <v>200</v>
@@ -3088,7 +3088,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>200</v>
+        <v>200000</v>
       </c>
       <c r="B17">
         <v>200</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>250</v>
+        <v>250000</v>
       </c>
       <c r="B18">
         <v>200</v>
@@ -3135,7 +3135,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>500</v>
+        <v>500000</v>
       </c>
       <c r="B19">
         <v>200</v>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E34" t="e">
-        <f t="shared" ref="E34:E65" si="3">((B34-C34)/1000)/D34</f>
+        <f t="shared" ref="E34:E60" si="3">((B34-C34)/1000)/D34</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F34" t="e">

</xml_diff>